<commit_message>
Files pushed 11:30 am Dec 19
</commit_message>
<xml_diff>
--- a/Markdown501/Roll Yield/Data/Corn Forward Curve Compare.xlsx
+++ b/Markdown501/Roll Yield/Data/Corn Forward Curve Compare.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20380"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jim\Dropbox\Teach\2021-2022\FRE 501\Roll Yield\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krishlim\OneDrive - UBC\Desktop\mfre\2021w-fre501\rollyield\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="10" documentId="11_A130F947BAA5B483C9124B340ED4F215002BCBA8" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{537C2C8A-887F-446D-8EA0-2A09940FE97C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7620" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="May 2021" sheetId="2" r:id="rId1"/>
@@ -64,7 +65,7 @@
     <definedName name="X_5">[1]Main!$E$3</definedName>
     <definedName name="Z">[1]Main!$E$6</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -211,40 +212,40 @@
     <t>Q8</t>
   </si>
   <si>
-    <t>Jul (near)</t>
-  </si>
-  <si>
-    <t>Sep (near)</t>
-  </si>
-  <si>
-    <t>Dec (near)</t>
-  </si>
-  <si>
-    <t>Mar (distant)</t>
-  </si>
-  <si>
-    <t>May (distant)</t>
-  </si>
-  <si>
-    <t>Jul (distant)</t>
-  </si>
-  <si>
-    <t>Sep (distant)</t>
-  </si>
-  <si>
-    <t>Dec (distant)</t>
-  </si>
-  <si>
     <t>July 2, 2020</t>
   </si>
   <si>
     <t>June 2, 2021</t>
+  </si>
+  <si>
+    <t>Jul_O</t>
+  </si>
+  <si>
+    <t>Sep_O</t>
+  </si>
+  <si>
+    <t>Dec_O</t>
+  </si>
+  <si>
+    <t>Mar_N</t>
+  </si>
+  <si>
+    <t>May_N</t>
+  </si>
+  <si>
+    <t>Jul_N</t>
+  </si>
+  <si>
+    <t>Sep_N</t>
+  </si>
+  <si>
+    <t>Dec_N</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
@@ -370,28 +371,28 @@
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>Jul (near)</c:v>
+                  <c:v>Jul_O</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Sep (near)</c:v>
+                  <c:v>Sep_O</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Dec (near)</c:v>
+                  <c:v>Dec_O</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Mar (distant)</c:v>
+                  <c:v>Mar_N</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>May (distant)</c:v>
+                  <c:v>May_N</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Jul (distant)</c:v>
+                  <c:v>Jul_N</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Sep (distant)</c:v>
+                  <c:v>Sep_N</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Dec (distant)</c:v>
+                  <c:v>Dec_N</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -465,28 +466,28 @@
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>Jul (near)</c:v>
+                  <c:v>Jul_O</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Sep (near)</c:v>
+                  <c:v>Sep_O</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Dec (near)</c:v>
+                  <c:v>Dec_O</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Mar (distant)</c:v>
+                  <c:v>Mar_N</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>May (distant)</c:v>
+                  <c:v>May_N</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Jul (distant)</c:v>
+                  <c:v>Jul_N</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Sep (distant)</c:v>
+                  <c:v>Sep_N</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Dec (distant)</c:v>
+                  <c:v>Dec_N</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -553,19 +554,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Mar (distant)</c:v>
+                  <c:v>Mar_N</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>May (distant)</c:v>
+                  <c:v>May_N</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Jul (distant)</c:v>
+                  <c:v>Jul_N</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Sep (distant)</c:v>
+                  <c:v>Sep_N</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Dec (distant)</c:v>
+                  <c:v>Dec_N</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -615,19 +616,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Mar (distant)</c:v>
+                  <c:v>Mar_N</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>May (distant)</c:v>
+                  <c:v>May_N</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Jul (distant)</c:v>
+                  <c:v>Jul_N</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Sep (distant)</c:v>
+                  <c:v>Sep_N</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Dec (distant)</c:v>
+                  <c:v>Dec_N</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -788,7 +789,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -892,7 +892,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1629,7 +1628,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1672,7 +1677,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1715,7 +1726,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -2209,21 +2226,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="P3" sqref="P3:Q14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="P3" t="s">
         <v>1</v>
       </c>
@@ -2231,7 +2248,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="P4" s="1">
         <v>44398</v>
       </c>
@@ -2239,7 +2256,7 @@
         <v>6.5724999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="P5" s="1">
         <v>44460</v>
       </c>
@@ -2247,7 +2264,7 @@
         <v>5.6849999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="P6" s="1">
         <v>44551</v>
       </c>
@@ -2255,7 +2272,7 @@
         <v>5.4024999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="P7" s="1">
         <v>44277</v>
       </c>
@@ -2263,7 +2280,7 @@
         <v>5.4625000000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="P8" s="1">
         <v>44338</v>
       </c>
@@ -2271,7 +2288,7 @@
         <v>5.4950000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="P9" s="1">
         <v>44399</v>
       </c>
@@ -2279,7 +2296,7 @@
         <v>5.4824999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="P10" s="1">
         <v>44461</v>
       </c>
@@ -2287,7 +2304,7 @@
         <v>4.9325000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="P11" s="1">
         <v>44552</v>
       </c>
@@ -2295,7 +2312,7 @@
         <v>4.7874999999999996</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="P12" s="1">
         <v>44278</v>
       </c>
@@ -2303,7 +2320,7 @@
         <v>4.8550000000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="P13" s="1">
         <v>44339</v>
       </c>
@@ -2311,7 +2328,7 @@
         <v>4.87</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="P14" s="1">
         <v>44400</v>
       </c>
@@ -2326,16 +2343,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="O1:P12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P2" sqref="P2:P9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="15:16" x14ac:dyDescent="0.3">
       <c r="O1" t="s">
         <v>1</v>
       </c>
@@ -2343,7 +2360,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="15:16" x14ac:dyDescent="0.3">
       <c r="O2" s="1">
         <v>44398</v>
       </c>
@@ -2351,7 +2368,7 @@
         <v>6.75</v>
       </c>
     </row>
-    <row r="3" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="15:16" x14ac:dyDescent="0.3">
       <c r="O3" s="1">
         <v>44460</v>
       </c>
@@ -2359,7 +2376,7 @@
         <v>5.9325000000000001</v>
       </c>
     </row>
-    <row r="4" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="15:16" x14ac:dyDescent="0.3">
       <c r="O4" s="1">
         <v>44551</v>
       </c>
@@ -2367,7 +2384,7 @@
         <v>5.7275</v>
       </c>
     </row>
-    <row r="5" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="15:16" x14ac:dyDescent="0.3">
       <c r="O5" s="1">
         <v>44277</v>
       </c>
@@ -2375,7 +2392,7 @@
         <v>5.7925000000000004</v>
       </c>
     </row>
-    <row r="6" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="15:16" x14ac:dyDescent="0.3">
       <c r="O6" s="1">
         <v>44338</v>
       </c>
@@ -2383,7 +2400,7 @@
         <v>5.8250000000000002</v>
       </c>
     </row>
-    <row r="7" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="15:16" x14ac:dyDescent="0.3">
       <c r="O7" s="1">
         <v>44399</v>
       </c>
@@ -2391,7 +2408,7 @@
         <v>5.8224999999999998</v>
       </c>
     </row>
-    <row r="8" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="15:16" x14ac:dyDescent="0.3">
       <c r="O8" s="1">
         <v>44461</v>
       </c>
@@ -2399,7 +2416,7 @@
         <v>5.17</v>
       </c>
     </row>
-    <row r="9" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="15:16" x14ac:dyDescent="0.3">
       <c r="O9" s="1">
         <v>44552</v>
       </c>
@@ -2407,7 +2424,7 @@
         <v>4.97</v>
       </c>
     </row>
-    <row r="10" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="15:16" x14ac:dyDescent="0.3">
       <c r="O10" s="1">
         <v>44278</v>
       </c>
@@ -2415,7 +2432,7 @@
         <v>5.03</v>
       </c>
     </row>
-    <row r="11" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="15:16" x14ac:dyDescent="0.3">
       <c r="O11" s="1">
         <v>44339</v>
       </c>
@@ -2423,7 +2440,7 @@
         <v>5.0575000000000001</v>
       </c>
     </row>
-    <row r="12" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="15:16" x14ac:dyDescent="0.3">
       <c r="O12" s="1">
         <v>44400</v>
       </c>
@@ -2438,16 +2455,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="A17" sqref="A17:D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2498,7 +2515,7 @@
         <v>3.4249999999999998</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>20200724</v>
       </c>
@@ -2540,7 +2557,7 @@
         <v>3.4350000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>20200724</v>
       </c>
@@ -2582,7 +2599,7 @@
         <v>3.5350000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>20200724</v>
       </c>
@@ -2624,7 +2641,7 @@
         <v>3.65</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>20200724</v>
       </c>
@@ -2666,7 +2683,7 @@
         <v>3.7075</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>20200724</v>
       </c>
@@ -2708,7 +2725,7 @@
         <v>3.7475000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>20200724</v>
       </c>
@@ -2750,7 +2767,7 @@
         <v>3.6775000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>20200724</v>
       </c>
@@ -2792,7 +2809,7 @@
         <v>3.74</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>20200724</v>
       </c>
@@ -2834,7 +2851,7 @@
         <v>3.8275000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>20200724</v>
       </c>
@@ -2876,7 +2893,7 @@
         <v>3.88</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>20200724</v>
       </c>
@@ -2918,7 +2935,7 @@
         <v>3.9175</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>20200724</v>
       </c>
@@ -2960,7 +2977,7 @@
         <v>3.8075000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>20200724</v>
       </c>
@@ -3002,7 +3019,7 @@
         <v>3.8125</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>20200724</v>
       </c>
@@ -3037,7 +3054,7 @@
         <v>381.25</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>20200724</v>
       </c>
@@ -3072,7 +3089,7 @@
         <v>397.5</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
         <v>19</v>
       </c>
@@ -3104,24 +3121,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:AJ44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.5703125" customWidth="1"/>
-    <col min="30" max="30" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.5546875" customWidth="1"/>
+    <col min="30" max="30" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:36" x14ac:dyDescent="0.3">
       <c r="C1" s="8" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
         <v>24</v>
@@ -3130,12 +3147,12 @@
         <v>25</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="2:36" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="2:36" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C2">
         <f>'July 2020'!Q1</f>
@@ -3146,9 +3163,9 @@
         <v>6.75</v>
       </c>
     </row>
-    <row r="3" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:36" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C3">
         <f>'July 2020'!Q2</f>
@@ -3159,9 +3176,9 @@
         <v>5.9325000000000001</v>
       </c>
     </row>
-    <row r="4" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:36" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C4">
         <f>'July 2020'!Q3</f>
@@ -3172,9 +3189,9 @@
         <v>5.7275</v>
       </c>
     </row>
-    <row r="5" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:36" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C5">
         <f>'July 2020'!Q4</f>
@@ -3185,9 +3202,9 @@
         <v>5.7925000000000004</v>
       </c>
     </row>
-    <row r="6" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:36" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C6">
         <f>'July 2020'!Q5</f>
@@ -3199,9 +3216,9 @@
         <v>5.8250000000000002</v>
       </c>
     </row>
-    <row r="7" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:36" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C7">
         <f>'July 2020'!Q6</f>
@@ -3211,9 +3228,9 @@
         <v>5.8224999999999998</v>
       </c>
     </row>
-    <row r="8" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:36" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C8">
         <f>'July 2020'!Q7</f>
@@ -3223,9 +3240,9 @@
         <v>5.17</v>
       </c>
     </row>
-    <row r="9" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:36" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C9">
         <f>'July 2020'!Q8</f>
@@ -3235,41 +3252,41 @@
         <v>4.97</v>
       </c>
     </row>
-    <row r="14" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:36" x14ac:dyDescent="0.3">
       <c r="AD14" s="4"/>
       <c r="AE14" s="5"/>
       <c r="AF14" s="5"/>
     </row>
-    <row r="16" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:36" x14ac:dyDescent="0.3">
       <c r="AH16" s="9"/>
       <c r="AI16" s="9"/>
       <c r="AJ16" s="9"/>
     </row>
-    <row r="18" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C25" s="3"/>
     </row>
-    <row r="32" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:30" x14ac:dyDescent="0.3">
       <c r="S32" s="9"/>
       <c r="T32" s="9"/>
       <c r="U32" s="9"/>
@@ -3281,7 +3298,7 @@
       <c r="AC32" s="9"/>
       <c r="AD32" s="9"/>
     </row>
-    <row r="33" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B33" s="5"/>
       <c r="C33" s="9" t="s">
         <v>26</v>
@@ -3317,7 +3334,7 @@
       <c r="AC33" s="5"/>
       <c r="AD33" s="5"/>
     </row>
-    <row r="34" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B34" s="5"/>
       <c r="C34" t="s">
         <v>22</v>
@@ -3369,7 +3386,7 @@
       <c r="AC34" s="6"/>
       <c r="AD34" s="6"/>
     </row>
-    <row r="35" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B35" s="5" t="s">
         <v>32</v>
       </c>
@@ -3427,7 +3444,7 @@
       <c r="AC35" s="6"/>
       <c r="AD35" s="6"/>
     </row>
-    <row r="36" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B36" s="5" t="s">
         <v>34</v>
       </c>
@@ -3485,7 +3502,7 @@
       <c r="AC36" s="6"/>
       <c r="AD36" s="6"/>
     </row>
-    <row r="37" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B37" s="5" t="s">
         <v>36</v>
       </c>
@@ -3543,7 +3560,7 @@
       <c r="AC37" s="6"/>
       <c r="AD37" s="6"/>
     </row>
-    <row r="38" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B38" s="5" t="s">
         <v>38</v>
       </c>
@@ -3601,7 +3618,7 @@
       <c r="AC38" s="6"/>
       <c r="AD38" s="6"/>
     </row>
-    <row r="39" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B39" s="5" t="s">
         <v>40</v>
       </c>
@@ -3659,7 +3676,7 @@
       <c r="AC39" s="6"/>
       <c r="AD39" s="6"/>
     </row>
-    <row r="40" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B40" s="5" t="s">
         <v>42</v>
       </c>
@@ -3694,7 +3711,7 @@
       <c r="AC40" s="9"/>
       <c r="AD40" s="9"/>
     </row>
-    <row r="41" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B41" s="5" t="s">
         <v>43</v>
       </c>
@@ -3729,7 +3746,7 @@
       <c r="AC41" s="5"/>
       <c r="AD41" s="5"/>
     </row>
-    <row r="42" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B42" s="5" t="s">
         <v>44</v>
       </c>
@@ -3765,7 +3782,7 @@
       <c r="AC42" s="6"/>
       <c r="AD42" s="6"/>
     </row>
-    <row r="43" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C43" s="3"/>
       <c r="I43" s="7"/>
       <c r="S43" s="6"/>
@@ -3779,7 +3796,7 @@
       <c r="AC43" s="6"/>
       <c r="AD43" s="6"/>
     </row>
-    <row r="44" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:30" x14ac:dyDescent="0.3">
       <c r="R44" t="s">
         <v>23</v>
       </c>

</xml_diff>